<commit_message>
BIS-997: New vocabularies to integrate views on the ELN
</commit_message>
<xml_diff>
--- a/core-plugin-openbis/dist/core-plugins/eln-lims-template-types/1/as/master-data/eln-types-template.xlsx
+++ b/core-plugin-openbis/dist/core-plugins/eln-lims-template-types/1/as/master-data/eln-types-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanf/Documents/sissource/openbis/core-plugin-openbis/dist/core-plugins/eln-lims-template-types/1/as/master-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3991F97-4BDA-9643-BBA7-BEE573743762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE363D6-2E12-6A4B-BC67-2D48250CB561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="500" windowWidth="48220" windowHeight="27220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELN_TYPES" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="99">
   <si>
     <t>SAMPLE_TYPE</t>
   </si>
@@ -295,6 +295,33 @@
   </si>
   <si>
     <t>Default Experiment</t>
+  </si>
+  <si>
+    <t>CONTROLLEDVOCABULARY</t>
+  </si>
+  <si>
+    <t>$DEFAULT_OBJECT_VIEW</t>
+  </si>
+  <si>
+    <t>$DEFAULT_OBJECT_VIEWS</t>
+  </si>
+  <si>
+    <t>Default object view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default view for objects </t>
+  </si>
+  <si>
+    <t>$DEFAULT_COLLECTION_VIEW</t>
+  </si>
+  <si>
+    <t>Default collection view</t>
+  </si>
+  <si>
+    <t>$DEFAULT_COLLECTION_VIEWS</t>
+  </si>
+  <si>
+    <t>Default view for experiments of the type collection</t>
   </si>
 </sst>
 </file>
@@ -304,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -351,6 +378,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -372,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +427,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,9 +744,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1009,8 +1047,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>31</v>
+      <c r="A15" t="s">
+        <v>91</v>
       </c>
       <c r="B15" s="6" t="b">
         <v>0</v>
@@ -1018,22 +1056,25 @@
       <c r="C15" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>33</v>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="b">
         <v>0</v>
@@ -1045,18 +1086,18 @@
         <v>16</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="6" t="b">
         <v>0</v>
@@ -1068,18 +1109,18 @@
         <v>16</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="6" t="b">
         <v>0</v>
@@ -1088,24 +1129,21 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="b">
         <v>0</v>
@@ -1117,13 +1155,13 @@
         <v>40</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>26</v>
@@ -1131,7 +1169,7 @@
     </row>
     <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B20" s="6" t="b">
         <v>0</v>
@@ -1143,13 +1181,13 @@
         <v>40</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>26</v>
@@ -1157,7 +1195,7 @@
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21" s="6" t="b">
         <v>0</v>
@@ -1169,21 +1207,21 @@
         <v>40</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B22" s="6" t="b">
         <v>0</v>
@@ -1191,25 +1229,25 @@
       <c r="C22" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>54</v>
+      <c r="D22" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" s="6" t="b">
         <v>0</v>
@@ -1221,13 +1259,13 @@
         <v>54</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>26</v>
@@ -1235,7 +1273,7 @@
     </row>
     <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" s="6" t="b">
         <v>0</v>
@@ -1244,16 +1282,16 @@
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>26</v>
@@ -1261,119 +1299,122 @@
     </row>
     <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="5" t="s">
+      <c r="B26" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="31" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B31" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>66</v>
       </c>
       <c r="B32" s="6" t="b">
         <v>0</v>
@@ -1385,18 +1426,18 @@
         <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H32" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="B33" s="6" t="b">
         <v>0</v>
@@ -1408,18 +1449,18 @@
         <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H33" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B34" s="6" t="b">
         <v>0</v>
@@ -1431,18 +1472,18 @@
         <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H34" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="B35" s="6" t="b">
         <v>0</v>
@@ -1450,22 +1491,25 @@
       <c r="C35" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>18</v>
+        <v>96</v>
+      </c>
+      <c r="F35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" t="s">
+        <v>97</v>
       </c>
       <c r="H35" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36" s="6" t="b">
         <v>0</v>
@@ -1477,18 +1521,18 @@
         <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="H36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B37" s="6" t="b">
         <v>0</v>
@@ -1500,18 +1544,18 @@
         <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B38" s="6" t="b">
         <v>0</v>
@@ -1520,24 +1564,21 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H38" t="s">
-        <v>42</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B39" s="6" t="b">
         <v>0</v>
@@ -1546,24 +1587,21 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H39" t="s">
-        <v>45</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B40" s="6" t="b">
         <v>0</v>
@@ -1575,21 +1613,21 @@
         <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H40" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
-        <v>53</v>
+      <c r="A41" t="s">
+        <v>73</v>
       </c>
       <c r="B41" s="6" t="b">
         <v>0</v>
@@ -1597,25 +1635,25 @@
       <c r="C41" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>54</v>
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>55</v>
+      <c r="H41" t="s">
+        <v>45</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>56</v>
+      <c r="A42" t="s">
+        <v>74</v>
       </c>
       <c r="B42" s="6" t="b">
         <v>0</v>
@@ -1623,17 +1661,17 @@
       <c r="C42" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>57</v>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" t="s">
+        <v>75</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H42" s="5" t="s">
-        <v>58</v>
+      <c r="H42" t="s">
+        <v>48</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>26</v>
@@ -1641,7 +1679,7 @@
     </row>
     <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B43" s="6" t="b">
         <v>0</v>
@@ -1649,15 +1687,17 @@
       <c r="C43" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="E43" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>26</v>
@@ -1665,131 +1705,181 @@
     </row>
     <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="B46" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F46" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="48" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="B52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="B53" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="4"/>
-    </row>
-    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="B56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>65</v>
       </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="B59" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D59" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E59" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D60" t="s">
         <v>89</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E60" s="4" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>